<commit_message>
link forms aula03 logica
</commit_message>
<xml_diff>
--- a/mecatronica/lp/frequencia.xlsx
+++ b/mecatronica/lp/frequencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wellington\senai2025\mecatronica\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28A4D92-D57E-47F2-A40D-10855EE0C218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D214A337-974B-445F-8E5C-2C03186BAE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{61FC206C-72CD-4264-B2AB-BE85D1DED9B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="21">
   <si>
     <t>Guilherme Assis Pereira</t>
   </si>
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C792F40-3E98-4415-93FE-BF383DE9D8A9}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
     <col min="6" max="33" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>45680</v>
       </c>
@@ -530,8 +530,11 @@
       <c r="E1" s="4">
         <v>45701</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4">
+        <v>45708</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -547,8 +550,11 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -564,8 +570,11 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -581,8 +590,11 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -598,8 +610,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -615,8 +630,11 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -632,8 +650,11 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,8 +670,11 @@
       <c r="E8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -666,8 +690,11 @@
       <c r="E9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -683,8 +710,11 @@
       <c r="E10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -700,8 +730,11 @@
       <c r="E11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -717,8 +750,11 @@
       <c r="E12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -734,8 +770,11 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -751,8 +790,11 @@
       <c r="E14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -768,8 +810,11 @@
       <c r="E15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -785,8 +830,11 @@
       <c r="E16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -802,8 +850,11 @@
       <c r="E17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -819,8 +870,11 @@
       <c r="E18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -836,8 +890,11 @@
       <c r="E19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -851,6 +908,9 @@
         <v>20</v>
       </c>
       <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>